<commit_message>
maga 2nd time push for programming
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse\Comcast_selenium_framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1141573-80F4-462C-8EF1-3FCA386A74F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D0291D-3819-4085-B6DA-478B39B36553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF1D8BEE-7F98-4F3E-B107-47791D2E9563}"/>
   </bookViews>
@@ -32,15 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Magaa</t>
-  </si>
-  <si>
-    <t>Long driver</t>
-  </si>
-  <si>
-    <t>lfjkhhkl</t>
+    <t>dooosraa</t>
   </si>
 </sst>
 </file>
@@ -392,27 +386,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F819852-9CC8-4AAE-B82A-07AB9C6839E7}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="1" max="1" width="66.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F11" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>